<commit_message>
proceed revised transportation schedule
</commit_message>
<xml_diff>
--- a/assets/excel/물량산정/물량산정엑셀로 올린것/여수학동 체크리스트-up.xlsx
+++ b/assets/excel/물량산정/물량산정엑셀로 올린것/여수학동 체크리스트-up.xlsx
@@ -58,15 +58,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>조정된 운송차수</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>기둥번호</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>운송차수계획(현재)</t>
+    <t>운송차수계획(13차)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>조정된 운송차수(12차)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -76,7 +76,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -213,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2298,7 +2298,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2328,10 +2328,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>